<commit_message>
Vet update to antidepressants
</commit_message>
<xml_diff>
--- a/RxNorm/Antidepressant/Same_Antidepressant_Medications.xlsx
+++ b/RxNorm/Antidepressant/Same_Antidepressant_Medications.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="415">
   <si>
     <t>rxcui</t>
   </si>
@@ -478,24 +478,6 @@
     <t>905172</t>
   </si>
   <si>
-    <t>859186</t>
-  </si>
-  <si>
-    <t>859190</t>
-  </si>
-  <si>
-    <t>859193</t>
-  </si>
-  <si>
-    <t>865206</t>
-  </si>
-  <si>
-    <t>865210</t>
-  </si>
-  <si>
-    <t>865214</t>
-  </si>
-  <si>
     <t>251201</t>
   </si>
   <si>
@@ -1060,24 +1042,6 @@
     <t>protriptyline hydrochloride 5 MG Oral Tablet</t>
   </si>
   <si>
-    <t>selegiline hydrochloride 5 MG Oral Capsule</t>
-  </si>
-  <si>
-    <t>selegiline hydrochloride 1.25 MG Disintegrating Oral Tablet</t>
-  </si>
-  <si>
-    <t>selegiline hydrochloride 5 MG Oral Tablet</t>
-  </si>
-  <si>
-    <t>24 HR selegiline 0.25 MG/HR Transdermal System</t>
-  </si>
-  <si>
-    <t>24 HR selegiline 0.375 MG/HR Transdermal System</t>
-  </si>
-  <si>
-    <t>24 HR selegiline 0.5 MG/HR Transdermal System</t>
-  </si>
-  <si>
     <t>sertraline 200 MG Oral Capsule</t>
   </si>
   <si>
@@ -1274,9 +1238,6 @@
   </si>
   <si>
     <t>protriptyline</t>
-  </si>
-  <si>
-    <t>selegiline</t>
   </si>
   <si>
     <t>sertraline</t>
@@ -1655,7 +1616,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1680,13 +1641,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D2" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1694,13 +1655,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1708,13 +1669,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D4" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1722,13 +1683,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D5" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1736,13 +1697,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D6" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1750,13 +1711,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C7" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D7" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1764,13 +1725,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D8" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1778,13 +1739,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D9" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1792,13 +1753,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D10" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1806,13 +1767,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D11" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1820,13 +1781,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D12" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1834,13 +1795,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D13" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1848,13 +1809,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D14" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1862,13 +1823,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D15" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1876,13 +1837,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D16" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1890,13 +1851,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C17" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D17" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1904,13 +1865,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D18" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1918,13 +1879,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D19" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1932,13 +1893,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C20" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D20" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1946,13 +1907,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D21" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1960,13 +1921,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D22" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1974,13 +1935,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C23" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D23" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1988,13 +1949,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C24" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D24" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2002,13 +1963,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C25" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D25" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2016,13 +1977,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C26" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D26" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2030,13 +1991,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C27" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D27" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2044,13 +2005,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C28" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D28" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2058,13 +2019,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C29" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D29" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2072,13 +2033,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D30" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2086,13 +2047,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C31" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D31" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2100,13 +2061,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D32" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2114,13 +2075,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C33" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D33" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2128,13 +2089,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C34" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D34" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2142,13 +2103,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D35" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2156,13 +2117,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D36" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2170,13 +2131,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C37" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D37" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2184,13 +2145,13 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C38" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D38" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2198,13 +2159,13 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C39" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D39" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2212,13 +2173,13 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D40" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2226,13 +2187,13 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D41" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2240,13 +2201,13 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C42" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D42" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2254,13 +2215,13 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D43" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2268,13 +2229,13 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C44" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D44" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2282,13 +2243,13 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C45" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D45" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2296,13 +2257,13 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C46" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D46" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2310,13 +2271,13 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C47" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D47" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2324,13 +2285,13 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C48" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D48" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2338,13 +2299,13 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C49" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D49" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2352,13 +2313,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C50" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D50" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2366,13 +2327,13 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C51" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D51" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2380,13 +2341,13 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C52" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D52" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2394,13 +2355,13 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C53" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D53" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2408,13 +2369,13 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C54" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D54" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2422,13 +2383,13 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C55" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D55" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2436,13 +2397,13 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C56" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D56" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2450,13 +2411,13 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C57" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D57" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2464,13 +2425,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C58" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D58" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2478,13 +2439,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D59" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2492,13 +2453,13 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C60" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D60" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2506,13 +2467,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C61" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D61" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2520,13 +2481,13 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C62" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D62" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2534,13 +2495,13 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C63" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D63" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2548,13 +2509,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C64" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D64" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2562,13 +2523,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C65" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D65" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2576,13 +2537,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C66" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D66" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2590,13 +2551,13 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C67" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D67" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2604,13 +2565,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C68" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D68" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2618,13 +2579,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
+        <v>380</v>
+      </c>
+      <c r="D69" t="s">
         <v>392</v>
-      </c>
-      <c r="D69" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2632,13 +2593,13 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C70" t="s">
+        <v>380</v>
+      </c>
+      <c r="D70" t="s">
         <v>392</v>
-      </c>
-      <c r="D70" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2646,13 +2607,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C71" t="s">
+        <v>380</v>
+      </c>
+      <c r="D71" t="s">
         <v>392</v>
-      </c>
-      <c r="D71" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2660,13 +2621,13 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C72" t="s">
+        <v>380</v>
+      </c>
+      <c r="D72" t="s">
         <v>392</v>
-      </c>
-      <c r="D72" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2674,13 +2635,13 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C73" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D73" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2688,13 +2649,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C74" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D74" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2702,13 +2663,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C75" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D75" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2716,13 +2677,13 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C76" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D76" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2730,13 +2691,13 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C77" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D77" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2744,13 +2705,13 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C78" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D78" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2758,13 +2719,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C79" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D79" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2772,13 +2733,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C80" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D80" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2786,13 +2747,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C81" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D81" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2800,13 +2761,13 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C82" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D82" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2814,13 +2775,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C83" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D83" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2828,13 +2789,13 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C84" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D84" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2842,13 +2803,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="C85" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D85" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2856,13 +2817,13 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C86" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D86" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2870,13 +2831,13 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C87" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D87" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2884,13 +2845,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C88" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D88" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2898,13 +2859,13 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C89" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D89" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2912,13 +2873,13 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C90" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D90" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2926,13 +2887,13 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C91" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D91" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2940,13 +2901,13 @@
         <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C92" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D92" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2954,13 +2915,13 @@
         <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C93" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D93" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2968,13 +2929,13 @@
         <v>96</v>
       </c>
       <c r="B94" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C94" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D94" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2982,13 +2943,13 @@
         <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C95" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D95" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2996,13 +2957,13 @@
         <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D96" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3010,13 +2971,13 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="C97" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D97" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3024,13 +2985,13 @@
         <v>100</v>
       </c>
       <c r="B98" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C98" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D98" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3038,13 +2999,13 @@
         <v>101</v>
       </c>
       <c r="B99" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C99" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D99" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3052,13 +3013,13 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D100" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3066,13 +3027,13 @@
         <v>103</v>
       </c>
       <c r="B101" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C101" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="D101" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3080,13 +3041,13 @@
         <v>104</v>
       </c>
       <c r="B102" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C102" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D102" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3094,13 +3055,13 @@
         <v>105</v>
       </c>
       <c r="B103" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C103" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D103" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3108,13 +3069,13 @@
         <v>106</v>
       </c>
       <c r="B104" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C104" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D104" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3122,13 +3083,13 @@
         <v>107</v>
       </c>
       <c r="B105" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C105" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D105" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3136,13 +3097,13 @@
         <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C106" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D106" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3150,13 +3111,13 @@
         <v>109</v>
       </c>
       <c r="B107" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C107" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D107" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3164,13 +3125,13 @@
         <v>110</v>
       </c>
       <c r="B108" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C108" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D108" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3178,13 +3139,13 @@
         <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C109" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D109" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3192,13 +3153,13 @@
         <v>112</v>
       </c>
       <c r="B110" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C110" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D110" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3206,13 +3167,13 @@
         <v>113</v>
       </c>
       <c r="B111" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C111" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D111" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3220,13 +3181,13 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C112" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D112" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3234,13 +3195,13 @@
         <v>115</v>
       </c>
       <c r="B113" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C113" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D113" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3248,13 +3209,13 @@
         <v>116</v>
       </c>
       <c r="B114" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C114" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D114" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3262,13 +3223,13 @@
         <v>117</v>
       </c>
       <c r="B115" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C115" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D115" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3276,13 +3237,13 @@
         <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C116" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D116" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3290,13 +3251,13 @@
         <v>119</v>
       </c>
       <c r="B117" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C117" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D117" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3304,13 +3265,13 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C118" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D118" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3318,13 +3279,13 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C119" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D119" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3332,13 +3293,13 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C120" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D120" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3346,13 +3307,13 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C121" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D121" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3360,13 +3321,13 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D122" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3374,13 +3335,13 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C123" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D123" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3388,13 +3349,13 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C124" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D124" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3402,13 +3363,13 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C125" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D125" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3416,13 +3377,13 @@
         <v>128</v>
       </c>
       <c r="B126" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C126" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D126" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3430,13 +3391,13 @@
         <v>129</v>
       </c>
       <c r="B127" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C127" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D127" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3444,13 +3405,13 @@
         <v>130</v>
       </c>
       <c r="B128" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C128" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D128" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3458,13 +3419,13 @@
         <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C129" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D129" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3472,13 +3433,13 @@
         <v>132</v>
       </c>
       <c r="B130" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C130" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D130" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3486,13 +3447,13 @@
         <v>133</v>
       </c>
       <c r="B131" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C131" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D131" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3500,13 +3461,13 @@
         <v>134</v>
       </c>
       <c r="B132" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C132" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D132" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3514,13 +3475,13 @@
         <v>135</v>
       </c>
       <c r="B133" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C133" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D133" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3528,13 +3489,13 @@
         <v>136</v>
       </c>
       <c r="B134" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C134" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D134" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3542,13 +3503,13 @@
         <v>137</v>
       </c>
       <c r="B135" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C135" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D135" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3556,13 +3517,13 @@
         <v>138</v>
       </c>
       <c r="B136" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C136" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D136" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3570,13 +3531,13 @@
         <v>139</v>
       </c>
       <c r="B137" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C137" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D137" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3584,13 +3545,13 @@
         <v>140</v>
       </c>
       <c r="B138" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C138" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D138" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3598,13 +3559,13 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C139" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D139" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3612,13 +3573,13 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C140" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D140" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3626,13 +3587,13 @@
         <v>143</v>
       </c>
       <c r="B141" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C141" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D141" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3640,13 +3601,13 @@
         <v>144</v>
       </c>
       <c r="B142" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C142" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D142" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3654,13 +3615,13 @@
         <v>145</v>
       </c>
       <c r="B143" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C143" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D143" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3668,13 +3629,13 @@
         <v>146</v>
       </c>
       <c r="B144" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C144" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D144" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3682,13 +3643,13 @@
         <v>147</v>
       </c>
       <c r="B145" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C145" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D145" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3696,13 +3657,13 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C146" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D146" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3710,13 +3671,13 @@
         <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C147" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D147" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3724,13 +3685,13 @@
         <v>150</v>
       </c>
       <c r="B148" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C148" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D148" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3738,13 +3699,13 @@
         <v>151</v>
       </c>
       <c r="B149" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C149" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D149" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3752,13 +3713,13 @@
         <v>152</v>
       </c>
       <c r="B150" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="C150" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D150" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3766,13 +3727,13 @@
         <v>153</v>
       </c>
       <c r="B151" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C151" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D151" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3780,13 +3741,13 @@
         <v>154</v>
       </c>
       <c r="B152" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C152" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D152" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3794,13 +3755,13 @@
         <v>155</v>
       </c>
       <c r="B153" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C153" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D153" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3808,13 +3769,13 @@
         <v>156</v>
       </c>
       <c r="B154" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C154" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D154" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3822,13 +3783,13 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C155" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D155" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3836,13 +3797,13 @@
         <v>158</v>
       </c>
       <c r="B156" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C156" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D156" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3850,13 +3811,13 @@
         <v>159</v>
       </c>
       <c r="B157" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C157" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D157" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3864,13 +3825,13 @@
         <v>160</v>
       </c>
       <c r="B158" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C158" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D158" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3878,13 +3839,13 @@
         <v>161</v>
       </c>
       <c r="B159" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C159" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D159" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3892,13 +3853,13 @@
         <v>162</v>
       </c>
       <c r="B160" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C160" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D160" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3906,13 +3867,13 @@
         <v>163</v>
       </c>
       <c r="B161" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C161" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D161" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3920,13 +3881,13 @@
         <v>164</v>
       </c>
       <c r="B162" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C162" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D162" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3934,13 +3895,13 @@
         <v>165</v>
       </c>
       <c r="B163" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C163" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D163" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3948,13 +3909,13 @@
         <v>166</v>
       </c>
       <c r="B164" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C164" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D164" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3962,13 +3923,13 @@
         <v>167</v>
       </c>
       <c r="B165" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C165" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D165" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3976,13 +3937,13 @@
         <v>168</v>
       </c>
       <c r="B166" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C166" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D166" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -3990,13 +3951,13 @@
         <v>169</v>
       </c>
       <c r="B167" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C167" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D167" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4004,13 +3965,13 @@
         <v>170</v>
       </c>
       <c r="B168" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C168" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D168" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4018,13 +3979,13 @@
         <v>171</v>
       </c>
       <c r="B169" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C169" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D169" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4032,13 +3993,13 @@
         <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C170" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D170" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4046,13 +4007,13 @@
         <v>173</v>
       </c>
       <c r="B171" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C171" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D171" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4060,13 +4021,13 @@
         <v>174</v>
       </c>
       <c r="B172" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C172" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D172" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4074,13 +4035,13 @@
         <v>175</v>
       </c>
       <c r="B173" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C173" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D173" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4088,13 +4049,13 @@
         <v>176</v>
       </c>
       <c r="B174" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C174" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D174" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4102,13 +4063,13 @@
         <v>177</v>
       </c>
       <c r="B175" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C175" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D175" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4116,13 +4077,13 @@
         <v>178</v>
       </c>
       <c r="B176" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C176" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D176" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4130,13 +4091,13 @@
         <v>179</v>
       </c>
       <c r="B177" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C177" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D177" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4144,13 +4105,13 @@
         <v>180</v>
       </c>
       <c r="B178" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C178" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D178" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4158,13 +4119,13 @@
         <v>181</v>
       </c>
       <c r="B179" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C179" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D179" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4172,13 +4133,13 @@
         <v>182</v>
       </c>
       <c r="B180" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C180" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D180" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4186,13 +4147,13 @@
         <v>183</v>
       </c>
       <c r="B181" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C181" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D181" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4200,13 +4161,13 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C182" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D182" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4214,13 +4175,13 @@
         <v>185</v>
       </c>
       <c r="B183" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C183" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D183" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4228,13 +4189,13 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C184" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D184" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4242,13 +4203,13 @@
         <v>187</v>
       </c>
       <c r="B185" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C185" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D185" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4256,13 +4217,13 @@
         <v>188</v>
       </c>
       <c r="B186" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="C186" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D186" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4270,13 +4231,13 @@
         <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C187" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="D187" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4284,13 +4245,13 @@
         <v>190</v>
       </c>
       <c r="B188" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C188" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="D188" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4298,97 +4259,13 @@
         <v>191</v>
       </c>
       <c r="B189" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="C189" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D189" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4">
-      <c r="A190" t="s">
-        <v>192</v>
-      </c>
-      <c r="B190" t="s">
-        <v>386</v>
-      </c>
-      <c r="C190" t="s">
-        <v>392</v>
-      </c>
-      <c r="D190" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" t="s">
-        <v>193</v>
-      </c>
-      <c r="B191" t="s">
-        <v>387</v>
-      </c>
-      <c r="C191" t="s">
-        <v>392</v>
-      </c>
-      <c r="D191" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4">
-      <c r="A192" t="s">
-        <v>194</v>
-      </c>
-      <c r="B192" t="s">
-        <v>388</v>
-      </c>
-      <c r="C192" t="s">
-        <v>392</v>
-      </c>
-      <c r="D192" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4">
-      <c r="A193" t="s">
-        <v>195</v>
-      </c>
-      <c r="B193" t="s">
-        <v>389</v>
-      </c>
-      <c r="C193" t="s">
-        <v>392</v>
-      </c>
-      <c r="D193" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4">
-      <c r="A194" t="s">
-        <v>196</v>
-      </c>
-      <c r="B194" t="s">
-        <v>390</v>
-      </c>
-      <c r="C194" t="s">
-        <v>392</v>
-      </c>
-      <c r="D194" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4">
-      <c r="A195" t="s">
-        <v>197</v>
-      </c>
-      <c r="B195" t="s">
-        <v>391</v>
-      </c>
-      <c r="C195" t="s">
-        <v>392</v>
-      </c>
-      <c r="D195" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>